<commit_message>
priority not working as a way to do precedence!
</commit_message>
<xml_diff>
--- a/net.akehurst.language.comparisons/results/results.xlsx
+++ b/net.akehurst.language.comparisons/results/results.xlsx
@@ -508,13 +508,517 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1473">
+  <fonts count="1585">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -7161,7 +7665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1473">
+  <cellXfs count="1585">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -8634,6 +9138,118 @@
     <xf numFmtId="0" fontId="1470" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1472" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1474" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1476" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1478" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1480" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1482" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1484" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1486" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1488" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1490" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1492" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1494" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1496" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1498" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1500" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1502" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1504" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1506" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1508" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1510" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1512" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1514" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1516" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1518" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1520" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1522" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1524" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1526" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1528" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1530" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1532" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1534" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1536" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1538" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1540" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1542" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1544" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1546" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1548" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1550" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1552" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1554" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1556" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1558" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1560" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1562" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1564" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1566" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1568" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1570" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1572" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1574" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1576" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1578" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1580" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1582" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1584" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
@@ -8665,262 +9281,262 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="n" s="954">
-        <v>0.0</v>
-      </c>
-      <c r="C2" t="n" s="956">
+      <c r="B2" t="n" s="1474">
+        <v>1.0</v>
+      </c>
+      <c r="C2" t="n" s="1476">
         <v>0.0</v>
       </c>
       <c r="D2" t="n">
-        <v>69.0</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="n" s="960">
-        <v>0.0</v>
-      </c>
-      <c r="C3" t="n" s="962">
-        <v>1.0</v>
+      <c r="B3" t="n" s="1480">
+        <v>0.0</v>
+      </c>
+      <c r="C3" t="n" s="1482">
+        <v>0.0</v>
       </c>
       <c r="D3" t="n">
-        <v>921.0</v>
+        <v>761.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="n" s="966">
-        <v>0.0</v>
-      </c>
-      <c r="C4" t="n" s="968">
+      <c r="B4" t="n" s="1486">
+        <v>0.0</v>
+      </c>
+      <c r="C4" t="n" s="1488">
         <v>0.0</v>
       </c>
       <c r="D4" t="n">
-        <v>48.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="n" s="972">
-        <v>0.0</v>
-      </c>
-      <c r="C5" t="n" s="974">
+      <c r="B5" t="n" s="1492">
+        <v>0.0</v>
+      </c>
+      <c r="C5" t="n" s="1494">
         <v>0.0</v>
       </c>
       <c r="D5" t="n">
-        <v>8741.0</v>
+        <v>9019.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="n" s="978">
-        <v>0.0</v>
-      </c>
-      <c r="C6" t="n" s="980">
-        <v>0.0</v>
-      </c>
-      <c r="D6" t="n" s="982">
-        <v>6219.0</v>
+      <c r="B6" t="n" s="1498">
+        <v>0.0</v>
+      </c>
+      <c r="C6" t="n" s="1500">
+        <v>0.0</v>
+      </c>
+      <c r="D6" t="n" s="1502">
+        <v>6304.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="n" s="984">
-        <v>0.0</v>
-      </c>
-      <c r="C7" t="n" s="986">
-        <v>0.0</v>
-      </c>
-      <c r="D7" t="n" s="988">
-        <v>1249.0</v>
+      <c r="B7" t="n" s="1504">
+        <v>0.0</v>
+      </c>
+      <c r="C7" t="n" s="1506">
+        <v>0.0</v>
+      </c>
+      <c r="D7" t="n" s="1508">
+        <v>1243.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="n" s="990">
-        <v>0.0</v>
-      </c>
-      <c r="C8" t="n" s="992">
-        <v>0.0</v>
-      </c>
-      <c r="D8" t="n" s="994">
-        <v>1481.0</v>
+      <c r="B8" t="n" s="1510">
+        <v>0.0</v>
+      </c>
+      <c r="C8" t="n" s="1512">
+        <v>0.0</v>
+      </c>
+      <c r="D8" t="n" s="1514">
+        <v>1066.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="n" s="996">
-        <v>0.0</v>
-      </c>
-      <c r="C9" t="n" s="998">
+      <c r="B9" t="n" s="1516">
+        <v>0.0</v>
+      </c>
+      <c r="C9" t="n" s="1518">
         <v>0.0</v>
       </c>
       <c r="D9" t="n">
-        <v>5497.0</v>
+        <v>5457.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="n" s="1002">
-        <v>0.0</v>
-      </c>
-      <c r="C10" t="n" s="1004">
+      <c r="B10" t="n" s="1522">
+        <v>1.0</v>
+      </c>
+      <c r="C10" t="n" s="1524">
         <v>0.0</v>
       </c>
       <c r="D10" t="n">
-        <v>1612.0</v>
+        <v>1609.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="n" s="1008">
-        <v>0.0</v>
-      </c>
-      <c r="C11" t="n" s="1010">
+      <c r="B11" t="n" s="1528">
+        <v>0.0</v>
+      </c>
+      <c r="C11" t="n" s="1530">
         <v>0.0</v>
       </c>
       <c r="D11" t="n">
-        <v>104.0</v>
+        <v>96.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="n" s="1014">
-        <v>0.0</v>
-      </c>
-      <c r="C12" t="n" s="1016">
+      <c r="B12" t="n" s="1534">
+        <v>0.0</v>
+      </c>
+      <c r="C12" t="n" s="1536">
         <v>0.0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="n" s="1020">
-        <v>0.0</v>
-      </c>
-      <c r="C13" t="n" s="1022">
-        <v>0.0</v>
-      </c>
-      <c r="D13" t="n" s="1024">
-        <v>3893.0</v>
+      <c r="B13" t="n" s="1540">
+        <v>0.0</v>
+      </c>
+      <c r="C13" t="n" s="1542">
+        <v>0.0</v>
+      </c>
+      <c r="D13" t="n" s="1544">
+        <v>3875.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="n" s="1026">
-        <v>0.0</v>
-      </c>
-      <c r="C14" t="n" s="1028">
+      <c r="B14" t="n" s="1546">
+        <v>0.0</v>
+      </c>
+      <c r="C14" t="n" s="1548">
         <v>0.0</v>
       </c>
       <c r="D14" t="n">
-        <v>162.0</v>
+        <v>147.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B15" t="n" s="1032">
-        <v>0.0</v>
-      </c>
-      <c r="C15" t="n" s="1034">
-        <v>0.0</v>
-      </c>
-      <c r="D15" t="n" s="1036">
-        <v>2929.0</v>
+      <c r="B15" t="n" s="1552">
+        <v>0.0</v>
+      </c>
+      <c r="C15" t="n" s="1554">
+        <v>0.0</v>
+      </c>
+      <c r="D15" t="n" s="1556">
+        <v>2857.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="n" s="1038">
-        <v>0.0</v>
-      </c>
-      <c r="C16" t="n" s="1040">
+      <c r="B16" t="n" s="1558">
+        <v>0.0</v>
+      </c>
+      <c r="C16" t="n" s="1560">
         <v>0.0</v>
       </c>
       <c r="D16" t="n">
-        <v>883.0</v>
+        <v>871.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="n" s="1044">
-        <v>0.0</v>
-      </c>
-      <c r="C17" t="n" s="1046">
+      <c r="B17" t="n" s="1564">
+        <v>0.0</v>
+      </c>
+      <c r="C17" t="n" s="1566">
         <v>0.0</v>
       </c>
       <c r="D17" t="n">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
         <v>20</v>
       </c>
-      <c r="B18" t="n" s="1050">
-        <v>0.0</v>
-      </c>
-      <c r="C18" t="n" s="1052">
+      <c r="B18" t="n" s="1570">
+        <v>1.0</v>
+      </c>
+      <c r="C18" t="n" s="1572">
         <v>0.0</v>
       </c>
       <c r="D18" t="n" s="1054">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="n" s="1056">
-        <v>0.0</v>
-      </c>
-      <c r="C19" t="n" s="1058">
+      <c r="B19" t="n" s="1576">
+        <v>0.0</v>
+      </c>
+      <c r="C19" t="n" s="1578">
         <v>0.0</v>
       </c>
       <c r="D19" t="n" s="1060">
-        <v>14235.0</v>
+        <v>32361.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="n" s="1062">
-        <v>0.0</v>
-      </c>
-      <c r="C20" t="n" s="1064">
+      <c r="B20" t="n" s="1582">
+        <v>0.0</v>
+      </c>
+      <c r="C20" t="n" s="1584">
         <v>0.0</v>
       </c>
       <c r="D20" t="n" s="1066">

</xml_diff>